<commit_message>
New UIDMatrix and ScenarioTemplate (HWP in more detail).
</commit_message>
<xml_diff>
--- a/ScenarioTemplate/ScenarioTemplate.xlsx
+++ b/ScenarioTemplate/ScenarioTemplate.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11014"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarip/Developer/GHGScenario/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D57565-2A97-A94E-90CD-5E69D0189552}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01F1905-F180-4D40-8A1B-86CB89B9072A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3400" yWindow="-23520" windowWidth="31780" windowHeight="15720" xr2:uid="{75C8E5C7-F74C-4D49-A81A-30A616B13E12}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{75C8E5C7-F74C-4D49-A81A-30A616B13E12}"/>
   </bookViews>
   <sheets>
     <sheet name="LandUse" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="69">
   <si>
     <t>Carbon stoc changes and other emissions by gases</t>
   </si>
@@ -202,6 +211,36 @@
   </si>
   <si>
     <t>TOTAL CO2 eq.</t>
+  </si>
+  <si>
+    <t>Sawnwood domestic</t>
+  </si>
+  <si>
+    <t>Sawnwood exported</t>
+  </si>
+  <si>
+    <t>Sawnwood total</t>
+  </si>
+  <si>
+    <t>Wood panels domestic</t>
+  </si>
+  <si>
+    <t>Wood panels exported</t>
+  </si>
+  <si>
+    <t>Wood panels total</t>
+  </si>
+  <si>
+    <t>Paper and paperboard domestic</t>
+  </si>
+  <si>
+    <t>Paper and paperboard exported</t>
+  </si>
+  <si>
+    <t>Paper and paperboard total</t>
+  </si>
+  <si>
+    <t>kt  C</t>
   </si>
 </sst>
 </file>
@@ -667,10 +706,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A3:BL126"/>
+  <dimension ref="A3:BL131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="BT72" sqref="BT72"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1365,343 +1404,373 @@
       </c>
     </row>
     <row r="61" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="32" t="s">
         <v>51</v>
       </c>
+      <c r="B61" s="32"/>
+      <c r="C61" s="32"/>
     </row>
     <row r="62" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="32">
         <v>27</v>
       </c>
-      <c r="B62" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C62" s="14" t="s">
-        <v>4</v>
+      <c r="B62" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="63" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="32">
         <v>28</v>
       </c>
-      <c r="B63" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>4</v>
+      <c r="B63" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" s="32" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="64" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="32">
+      <c r="A64" s="32"/>
+      <c r="B64" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="32">
         <v>29</v>
       </c>
-      <c r="B64" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C64" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C65" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="32">
+        <v>30</v>
+      </c>
+      <c r="B66" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="32"/>
+      <c r="B67" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="32">
+        <v>31</v>
+      </c>
+      <c r="B68" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="32">
+        <v>32</v>
+      </c>
+      <c r="B69" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="32"/>
+      <c r="B70" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="32"/>
+      <c r="B71" s="32" t="s">
         <v>55</v>
       </c>
-      <c r="C65" s="14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
+      <c r="C71" s="32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B72" s="4" t="s">
+    <row r="77" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B77" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B73" s="5" t="s">
+    <row r="78" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B78" s="5" t="s">
         <v>3</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B74" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B75" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B76" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B77" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B78" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="79" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B79" s="4" t="s">
-        <v>10</v>
+      <c r="B79" s="5" t="s">
+        <v>5</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B80" s="16" t="s">
+    <row r="80" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B81" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B83" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B84" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B85" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C80" s="15" t="s">
+      <c r="C85" s="15" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="7" t="s">
+    <row r="87" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B83" s="8" t="s">
+    <row r="88" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B88" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="C83" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B84" s="8" t="s">
+      <c r="C88" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B89" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C84" s="7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B85" s="18" t="s">
+      <c r="C89" s="7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B90" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C85" s="17" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="9" t="s">
+      <c r="C90" s="17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="88" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B88" s="9" t="s">
+    <row r="93" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B93" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C88" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B89" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C89" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B90" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C90" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B91" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C91" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B92" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C92" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B93" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C93" s="19" t="s">
+      <c r="C93" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="94" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B94" s="9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C94" s="9" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="95" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B95" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B96" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C96" s="19" t="s">
+    <row r="95" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B95" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C95" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B96" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C96" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B97" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B98" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C98" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B99" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B100" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C100" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B101" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C101" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B102" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C97" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B98" s="9" t="s">
+      <c r="C102" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B103" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C98" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B99" s="19" t="s">
+      <c r="C103" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B104" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C99" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="11" t="s">
+      <c r="C104" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="102" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B102" s="20" t="s">
+    <row r="107" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B107" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C102" s="20" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="12" t="s">
+      <c r="C107" s="20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="105" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B105" s="12" t="s">
+    <row r="110" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B110" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C105" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B106" s="12" t="s">
+      <c r="C110" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B111" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C106" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B107" s="21" t="s">
+      <c r="C111" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B112" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C107" s="21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="13" t="s">
+      <c r="C112" s="21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="110" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B110" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="C110" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B111" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C111" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B112" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C112" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B113" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="C113" s="22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="115" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B115" s="13" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C115" s="13" t="s">
         <v>56</v>
@@ -1709,7 +1778,7 @@
     </row>
     <row r="116" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B116" s="13" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C116" s="13" t="s">
         <v>56</v>
@@ -1717,7 +1786,7 @@
     </row>
     <row r="117" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B117" s="13" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C117" s="13" t="s">
         <v>56</v>
@@ -1725,51 +1794,84 @@
     </row>
     <row r="118" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B118" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="C118" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="120" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B120" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C120" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B121" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C121" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B122" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C122" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B123" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C118" s="22" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="14" t="s">
+      <c r="C123" s="22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="121" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B121" s="14" t="s">
+    <row r="126" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B126" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C121" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="122" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B122" s="14" t="s">
+      <c r="C126" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B127" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C122" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="123" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B123" s="14" t="s">
+      <c r="C127" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B128" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C123" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="124" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B124" s="23" t="s">
+      <c r="C128" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B129" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="C124" s="23" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="24" t="s">
+      <c r="C129" s="23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="24" t="s">
         <v>58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New single Scenario template excel file that will contain all templates for output. Currently  UIDMatrix and LandUse.
</commit_message>
<xml_diff>
--- a/ScenarioTemplate/ScenarioTemplate.xlsx
+++ b/ScenarioTemplate/ScenarioTemplate.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarip/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarip/Developer/GHGInventory/GHG2019/lukeghg/ScenarioTemplate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B01F1905-F180-4D40-8A1B-86CB89B9072A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE7BD5E5-1884-BB4F-8563-86F8DE4D63CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{75C8E5C7-F74C-4D49-A81A-30A616B13E12}"/>
   </bookViews>
   <sheets>
-    <sheet name="LandUse" sheetId="1" r:id="rId1"/>
+    <sheet name="UIDMatrix" sheetId="2" r:id="rId1"/>
+    <sheet name="LandUse" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="219">
   <si>
     <t>Carbon stoc changes and other emissions by gases</t>
   </si>
@@ -241,6 +242,456 @@
   </si>
   <si>
     <t>kt  C</t>
+  </si>
+  <si>
+    <t>FL-FL</t>
+  </si>
+  <si>
+    <t>CL-FL</t>
+  </si>
+  <si>
+    <t>GL-FL</t>
+  </si>
+  <si>
+    <t>WLpeat-FL</t>
+  </si>
+  <si>
+    <t>WLother-FL</t>
+  </si>
+  <si>
+    <t>SE-FL</t>
+  </si>
+  <si>
+    <t>CL-CL</t>
+  </si>
+  <si>
+    <t>FL-CL</t>
+  </si>
+  <si>
+    <t>GL-CL</t>
+  </si>
+  <si>
+    <t>WLpeat-CL</t>
+  </si>
+  <si>
+    <t>WLother-CL</t>
+  </si>
+  <si>
+    <t>SE-CL</t>
+  </si>
+  <si>
+    <t>GL-GL</t>
+  </si>
+  <si>
+    <t>FL-GL</t>
+  </si>
+  <si>
+    <t>CL-GL</t>
+  </si>
+  <si>
+    <t>WLPeat-GL</t>
+  </si>
+  <si>
+    <t>WLother-GL</t>
+  </si>
+  <si>
+    <t>SE-GL</t>
+  </si>
+  <si>
+    <t>WL-WL(peatextraction)</t>
+  </si>
+  <si>
+    <t>WLother-WLpeat</t>
+  </si>
+  <si>
+    <t>FL-WLpeat</t>
+  </si>
+  <si>
+    <t>CL-WLpeat</t>
+  </si>
+  <si>
+    <t>GL-WLpeat</t>
+  </si>
+  <si>
+    <t>WL-WL(flooded)</t>
+  </si>
+  <si>
+    <t>FL-WLflooded</t>
+  </si>
+  <si>
+    <t>CL-WLflooded</t>
+  </si>
+  <si>
+    <t>GL-WLflooded</t>
+  </si>
+  <si>
+    <t>SE-WLflooded</t>
+  </si>
+  <si>
+    <t>OL-WLflooded</t>
+  </si>
+  <si>
+    <t>WL-WL(other)</t>
+  </si>
+  <si>
+    <t>WLpeat-WLother</t>
+  </si>
+  <si>
+    <t>FL-WLother</t>
+  </si>
+  <si>
+    <t>CL-WLother</t>
+  </si>
+  <si>
+    <t>GL-WLother</t>
+  </si>
+  <si>
+    <t>SE-SE</t>
+  </si>
+  <si>
+    <t>FL-SE</t>
+  </si>
+  <si>
+    <t>CL-SE</t>
+  </si>
+  <si>
+    <t>GL-SE</t>
+  </si>
+  <si>
+    <t>WLpeat-SE</t>
+  </si>
+  <si>
+    <t>WLother-SE</t>
+  </si>
+  <si>
+    <t>4A48C2F0-02C0-4EAB-8547-6A109929DDCD</t>
+  </si>
+  <si>
+    <t>020F0D40-E0CE-4AA7-B393-EAD6EADCEA9F</t>
+  </si>
+  <si>
+    <t>CB4FD2B9-6469-4A9B-9F06-B6F1A60C7B15</t>
+  </si>
+  <si>
+    <t>82E1F01F-68F4-46A3-867C-DA9C03481B2D</t>
+  </si>
+  <si>
+    <t>BFFBD46B-1FA4-4B93-84F8-61D970DCC5B1</t>
+  </si>
+  <si>
+    <t>176984AA-39DD-46BD-8783-2632BEF3C520</t>
+  </si>
+  <si>
+    <t>36CD6D26-94F4-4BDA-9111-5550B936E473</t>
+  </si>
+  <si>
+    <t>3F56BC8A-08E4-45CA-B1F7-8DAA14BE39C1</t>
+  </si>
+  <si>
+    <t>942BC69D-81D0-40F7-B034-DED89D2D4E00</t>
+  </si>
+  <si>
+    <t>2F5B1083-7134-4982-9FBC-238D55BFB41F</t>
+  </si>
+  <si>
+    <t>9268C483-1CDF-492B-A0CC-510A18787438</t>
+  </si>
+  <si>
+    <t>53255AB3-3284-479F-9451-7AA403AC0C99</t>
+  </si>
+  <si>
+    <t>96E8D24F-CBF5-4E09-BD19-D240F3DAEC67</t>
+  </si>
+  <si>
+    <t>29C9BDB9-5F4B-425C-AC6F-568A6BA18E5A</t>
+  </si>
+  <si>
+    <t>BB8A06DB-3524-4658-B3F4-39C8B3E3B9C4</t>
+  </si>
+  <si>
+    <t>E1B2A0CF-5F9F-445E-9715-C274A0CD4A26</t>
+  </si>
+  <si>
+    <t>406DBCA1-70FC-43C8-B338-C7A3EC027D60</t>
+  </si>
+  <si>
+    <t>383D214A-F102-4D0E-879B-B3F9E0339487</t>
+  </si>
+  <si>
+    <t>1B14CBDF-9649-4F68-B6FC-5118CED43F9E</t>
+  </si>
+  <si>
+    <t>ACCCE368-38E5-4BC7-A807-99DDAC520BBA</t>
+  </si>
+  <si>
+    <t>0A0CAA48-DB6F-412A-AFBD-8F078B1AF8A6</t>
+  </si>
+  <si>
+    <t>8B60CCEA-6FB6-49EC-A94E-AAC77C144727</t>
+  </si>
+  <si>
+    <t>2398E95A-4527-434A-9503-BF0E9FD260A9</t>
+  </si>
+  <si>
+    <t>FFD8E79B-1DA0-4399-910A-6E875F1A8F58</t>
+  </si>
+  <si>
+    <t>CB120EB8-E3C5-4A9D-948A-84800B40BB85</t>
+  </si>
+  <si>
+    <t>BEFED697-594C-4A84-8732-583E6A28379F</t>
+  </si>
+  <si>
+    <t>892E3E41-F618-4A95-844A-8FDF9A6FBFA5</t>
+  </si>
+  <si>
+    <t>D2528CC8-D398-422B-AEBA-27CE5A44091F</t>
+  </si>
+  <si>
+    <t>7C6816AA-0A8A-434B-84CD-62A1D52D3E88</t>
+  </si>
+  <si>
+    <t>EC5492F0-F9E4-4C2A-B994-585206486EBB</t>
+  </si>
+  <si>
+    <t>54D18A8E-B90E-4521-93AB-E8599CA5AE29</t>
+  </si>
+  <si>
+    <t>788519B8-6B25-4D79-A20B-D05E20407DEE</t>
+  </si>
+  <si>
+    <t>83B4EACE-21F0-44BF-8CA6-87E9720CCC7B</t>
+  </si>
+  <si>
+    <t>FE5FFEBE-E5C7-43A1-8DD8-31FF82A48F4B</t>
+  </si>
+  <si>
+    <t>E3719388-E913-43D0-8346-1B13D6663079</t>
+  </si>
+  <si>
+    <t>EB8699FD-1FAA-4739-8A01-F450C5097C54</t>
+  </si>
+  <si>
+    <t>DB6253EB-8660-4C1C-B880-10991D8E2DC5</t>
+  </si>
+  <si>
+    <t>810E194F-0D38-4486-8A88-96ACF87C2059</t>
+  </si>
+  <si>
+    <t>197C9403-609C-45DA-9A25-A0AD0BBA5930</t>
+  </si>
+  <si>
+    <t>80DA0459-04A7-494B-960D-74CA4BC2EAE1</t>
+  </si>
+  <si>
+    <t>6E9B1091-9498-487A-8C33-268D053181AA</t>
+  </si>
+  <si>
+    <t>33B17FCF-CEF0-4C52-A083-41E77975CC17</t>
+  </si>
+  <si>
+    <t>9CD08E1A-B433-497D-9209-EC017CA23724</t>
+  </si>
+  <si>
+    <t>B3F95305-ACF3-4064-A83E-705F560B39C8</t>
+  </si>
+  <si>
+    <t>8F57EF8B-E304-4EF0-8EC6-0FC6E8C2CDB0</t>
+  </si>
+  <si>
+    <t>E396B346-95B8-4F15-B0DD-AF88CD396A1D</t>
+  </si>
+  <si>
+    <t>48E78285-3774-46F3-AEBC-1F02736B1869</t>
+  </si>
+  <si>
+    <t>A4DB34A0-1847-401A-92BA-7CCE37611F1A</t>
+  </si>
+  <si>
+    <t>334088D5-54BD-44A2-A0EA-EFDD842DB36C</t>
+  </si>
+  <si>
+    <t>D92DA8FD-6AF2-44AE-83B2-C5994F5B0B8D</t>
+  </si>
+  <si>
+    <t>B34584B9-54FC-436F-9750-4D4E604DBDAB</t>
+  </si>
+  <si>
+    <t>C9699E83-31D7-400A-82F5-07DA80E995E9</t>
+  </si>
+  <si>
+    <t>CED9F314-185E-4B57-A302-3CEA41396C3D</t>
+  </si>
+  <si>
+    <t>6FAE66FC-C7F1-4721-BB8E-37A0830465E3</t>
+  </si>
+  <si>
+    <t>74FDB2BF-3FC6-4EB3-A1FD-F580F27CAC1A</t>
+  </si>
+  <si>
+    <t>341291A3-1CF1-4F57-98F2-3E986BEA3AFA</t>
+  </si>
+  <si>
+    <t>0C26CC53-5EEB-41F2-ABCF-8651816E847E</t>
+  </si>
+  <si>
+    <t>1632C1F2-832E-48D5-BA76-AA1DFAA643DC</t>
+  </si>
+  <si>
+    <t>BD9A7BB8-BBAA-47A5-9437-0F5517385FCE</t>
+  </si>
+  <si>
+    <t>5E64A07B-D172-42ED-8E28-0BAA407A9D59</t>
+  </si>
+  <si>
+    <t>4CA589AF-132A-4C1E-AAFE-FF384EABE789</t>
+  </si>
+  <si>
+    <t>661092F5-C566-4018-8792-41A7A3FED14C</t>
+  </si>
+  <si>
+    <t>758A489C-2516-4828-9DD7-DAA8C3FE2BAD</t>
+  </si>
+  <si>
+    <t>846E5F70-532C-4787-BBF3-5458B7BA2D5D</t>
+  </si>
+  <si>
+    <t>F6FB5D56-CF24-4A98-A516-A870BF67244A</t>
+  </si>
+  <si>
+    <t>41EB6051-3F79-4920-8331-0563481BC899</t>
+  </si>
+  <si>
+    <t>3B50B4A3-3C70-4ADC-8C0E-F8186DE147F2</t>
+  </si>
+  <si>
+    <t>EFEFA92B-496F-4805-9CDB-E6EB7A9C779B</t>
+  </si>
+  <si>
+    <t>A9A40D5A-95E7-47DF-8D15-CA9EF8916317</t>
+  </si>
+  <si>
+    <t>6B9C03D8-C39C-439D-993E-0F444F1EB30E</t>
+  </si>
+  <si>
+    <t>3F22874A-DA26-43B4-9D5E-DB968F0025C4</t>
+  </si>
+  <si>
+    <t>0E97BE1E-C32F-4C75-AB79-A3B8893CB7FE</t>
+  </si>
+  <si>
+    <t>7F43C0C7-8720-48A3-A4E6-E786A3848829</t>
+  </si>
+  <si>
+    <t>D0CD1135-8684-4AA6-A5B6-D4838AA51401</t>
+  </si>
+  <si>
+    <t>1F66B5AA-2CE8-4AC7-98B8-D1225EB7908E</t>
+  </si>
+  <si>
+    <t>E45E4D33-EF70-44B3-B677-411E0AE64D26</t>
+  </si>
+  <si>
+    <t>D25586E2-DC67-4941-B692-EF1D721E3E43</t>
+  </si>
+  <si>
+    <t>3EC71220-A20F-4D17-9E21-61052B40C018</t>
+  </si>
+  <si>
+    <t>FA5944EB-397A-4A9F-B1AB-621F095589D9</t>
+  </si>
+  <si>
+    <t>43107214-F52D-49AB-8D60-BB5A547BE291</t>
+  </si>
+  <si>
+    <t>9C84D2FE-B631-4004-829D-D61688D50086</t>
+  </si>
+  <si>
+    <t>D4126FA3-991C-4253-A5D9-E1E61C0BC9D5</t>
+  </si>
+  <si>
+    <t>6294235D-9C28-4AA3-89EF-7FF6A9EE6E68</t>
+  </si>
+  <si>
+    <t>375196C2-F23E-431E-9002-D4F9F131F75B</t>
+  </si>
+  <si>
+    <t>07707982-3317-46B1-AEA8-C0EBFEDA37F0</t>
+  </si>
+  <si>
+    <t>6CD89939-66E5-432F-8ADC-3D30C6F27776</t>
+  </si>
+  <si>
+    <t>D328C711-A441-4587-B515-B67E3B024FE2</t>
+  </si>
+  <si>
+    <t>26C39115-0D31-4A9D-A05B-6A9514813B84</t>
+  </si>
+  <si>
+    <t>7BB50E49-6297-4259-B504-A79DB85FA7E4</t>
+  </si>
+  <si>
+    <t>2EFF9018-A46A-4981-8D9C-DA517A310E7B</t>
+  </si>
+  <si>
+    <t>33640199-E4E9-4FAB-BE6F-6562C740009A</t>
+  </si>
+  <si>
+    <t>D9244D4E-A8DE-4DE8-8471-19DED97E95F0</t>
+  </si>
+  <si>
+    <t>1FDFE900-D9C3-44C5-9CCE-2AA4B6713DBB</t>
+  </si>
+  <si>
+    <t>E82036FA-99A3-4048-9B1F-5EC104BA0337</t>
+  </si>
+  <si>
+    <t>860D7B59-2124-4518-A98E-A9BA913F9118</t>
+  </si>
+  <si>
+    <t>B598E180-C1C5-492A-B7FA-C0FAB7816050</t>
+  </si>
+  <si>
+    <t>7CC2DF97-BECD-4191-A3B1-FBB01FF83D43</t>
+  </si>
+  <si>
+    <t>109C3AB7-0077-4367-8C74-E2467ACE7D16</t>
+  </si>
+  <si>
+    <t>87FC6342-FA45-4030-89E6-0E02A2BFC648</t>
+  </si>
+  <si>
+    <t>A5505411-C5E5-431C-BB58-25E152436833</t>
+  </si>
+  <si>
+    <t>6B7A581C-6A5E-4A77-86C9-FBB3BDEFC87E</t>
+  </si>
+  <si>
+    <t>29D1D560-ACF2-487D-9AF0-291BF6750BE0</t>
+  </si>
+  <si>
+    <t>D8ECB802-B474-4EFD-8A83-0BA019E9B019</t>
+  </si>
+  <si>
+    <t>283CB017-2D3E-4817-AFAB-CC3D885151AB</t>
+  </si>
+  <si>
+    <t>0B29C52E-CF04-46A9-AF23-BA996645E547</t>
+  </si>
+  <si>
+    <t>054E0C6F-5E84-4411-9022-B04049A2C6D0</t>
+  </si>
+  <si>
+    <t>CA184B1C-EB7C-42CB-897C-57AC319EAF39</t>
+  </si>
+  <si>
+    <t>42476E95-C4C0-4787-8E7B-2CDA36458710</t>
+  </si>
+  <si>
+    <t>185C43A5-D840-460E-8163-8B2F7BBB952C</t>
+  </si>
+  <si>
+    <t>3BBB8E1F-6E69-4551-A0F4-527BFBBBDBFB</t>
   </si>
 </sst>
 </file>
@@ -345,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -389,6 +840,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -702,13 +1154,1178 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03176DFC-C103-5847-A7A5-63D91BF465BB}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A3:AP130"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.6640625" customWidth="1"/>
+    <col min="5" max="5" width="6.5" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="6.5" customWidth="1"/>
+    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:42" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="5" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="X5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z5" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA5" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="AD5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE5" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="AJ5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AK5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AL5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AM5" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AN5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AO5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AP5" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="26">
+        <v>1</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="I9" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="T9" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="26">
+        <v>2</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="I10" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="O10" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="W10" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="X10" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y10" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA10" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="AB10" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="AC10" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH10" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="AJ10" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="AL10" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="AM10" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="AN10" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="26"/>
+      <c r="B11" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="26">
+        <v>3</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="W12" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AL12" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="26">
+        <v>4</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="26">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>150</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="K14" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="AL14" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="26">
+        <v>6</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="26" t="s">
+        <v>166</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="Q15" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="T15" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="U15" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="V15" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="W15" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="X15" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="Y15" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="Z15" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="AA15" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB15" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="AC15" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="AD15" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="AE15" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="AF15" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AG15" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="AH15" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="AJ15" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="27">
+        <v>7</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="27">
+        <v>8</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="27"/>
+      <c r="B21" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="28">
+        <v>9</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="U24" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="AF24" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="28">
+        <v>10</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="U25" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="AF25" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="28"/>
+      <c r="B26" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="28">
+        <v>11</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="28">
+        <v>12</v>
+      </c>
+      <c r="B28" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="28"/>
+      <c r="B29" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="28">
+        <v>13</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="28">
+        <v>14</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="28"/>
+      <c r="B32" s="9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="28">
+        <v>15</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="28">
+        <v>16</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="28"/>
+      <c r="B35" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="29">
+        <v>17</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>201</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>204</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="N38" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="P38" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q38" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="R38" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="T38" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="AL38" s="11" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="40" spans="1:38" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:38" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="30">
+        <v>18</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:38" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="30">
+        <v>19</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:38" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="30">
+        <v>20</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:38" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:38" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="31">
+        <v>21</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:38" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="31">
+        <v>22</v>
+      </c>
+      <c r="B47" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:38" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="31">
+        <v>23</v>
+      </c>
+      <c r="B48" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="31"/>
+      <c r="B49" s="13" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="31"/>
+    </row>
+    <row r="51" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="31">
+        <v>24</v>
+      </c>
+      <c r="B51" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="31">
+        <v>25</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="31">
+        <v>26</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B56" s="13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B57" s="13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="B61" s="32"/>
+      <c r="C61" s="32"/>
+    </row>
+    <row r="62" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="32">
+        <v>27</v>
+      </c>
+      <c r="B62" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="C62" s="32" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="32">
+        <v>28</v>
+      </c>
+      <c r="B63" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" s="32" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="32"/>
+      <c r="B64" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" s="32"/>
+    </row>
+    <row r="65" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="32">
+        <v>29</v>
+      </c>
+      <c r="B65" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C65" s="32" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="32">
+        <v>30</v>
+      </c>
+      <c r="B66" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="C66" s="32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="32"/>
+      <c r="B67" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C67" s="32"/>
+    </row>
+    <row r="68" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="32">
+        <v>31</v>
+      </c>
+      <c r="B68" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C68" s="32" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="32">
+        <v>32</v>
+      </c>
+      <c r="B69" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69" s="32" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="32"/>
+      <c r="B70" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C70" s="32"/>
+    </row>
+    <row r="71" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="32"/>
+      <c r="B71" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C71" s="32"/>
+    </row>
+    <row r="73" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B76" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B77" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B78" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B79" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B81" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B82" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B83" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B84" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B87" s="8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B88" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B89" s="18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B92" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B93" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B94" s="19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B95" s="9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B96" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B97" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B98" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B99" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B100" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B101" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B102" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B103" s="19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B106" s="20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B109" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B110" s="12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B111" s="21" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B114" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B115" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B116" s="13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B117" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="119" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B119" s="13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B120" s="13" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B121" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B122" s="22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B125" s="14" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B126" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B127" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B128" s="23" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="24" t="s">
+        <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6079F9EC-21D7-7841-A622-15AA8E507E07}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A3:BL131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+    <sheetView topLeftCell="A48" workbookViewId="0">
       <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Year 2023 improved UID Matrix
</commit_message>
<xml_diff>
--- a/ScenarioTemplate/ScenarioTemplate.xlsx
+++ b/ScenarioTemplate/ScenarioTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarip/Developer/GHGInventory/GHG2019/lukeghg/ScenarioTemplate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Luke\GHG\skenaariot\kehitys\tietojen siirto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8598340A-8B39-1B4D-904F-9511A49E3A56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9B4B45-6C7E-4CD6-86A9-5E5879AA6E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" activeTab="2" xr2:uid="{75C8E5C7-F74C-4D49-A81A-30A616B13E12}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75C8E5C7-F74C-4D49-A81A-30A616B13E12}"/>
   </bookViews>
   <sheets>
     <sheet name="UIDMatrix" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="295">
   <si>
     <t>Carbon stoc changes and other emissions by gases</t>
   </si>
@@ -629,18 +629,6 @@
     <t>26C39115-0D31-4A9D-A05B-6A9514813B84</t>
   </si>
   <si>
-    <t>7BB50E49-6297-4259-B504-A79DB85FA7E4</t>
-  </si>
-  <si>
-    <t>2EFF9018-A46A-4981-8D9C-DA517A310E7B</t>
-  </si>
-  <si>
-    <t>33640199-E4E9-4FAB-BE6F-6562C740009A</t>
-  </si>
-  <si>
-    <t>D9244D4E-A8DE-4DE8-8471-19DED97E95F0</t>
-  </si>
-  <si>
     <t>1FDFE900-D9C3-44C5-9CCE-2AA4B6713DBB</t>
   </si>
   <si>
@@ -759,6 +747,180 @@
   </si>
   <si>
     <t>WLflooded-FL</t>
+  </si>
+  <si>
+    <t>4F79582F-31DB-41D4-966D-9DBCD04B722A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">96022841-C27D-42CF-8EE3-0D1A5437AD6B </t>
+  </si>
+  <si>
+    <t>92DFB34F-5B75-4BCB-A758-7F346C1E918D</t>
+  </si>
+  <si>
+    <t>DAA0FB40-3EE2-4BB6-AE86-8C8BE148216B</t>
+  </si>
+  <si>
+    <t>A77C393E-254E-47A7-AA03-0D823A8E8C9D</t>
+  </si>
+  <si>
+    <t>22DBD636-5D80-4C41-AD31-CB2CA289CAEA</t>
+  </si>
+  <si>
+    <t>C7587797-74A3-4CBB-A0FA-207D86FEE948</t>
+  </si>
+  <si>
+    <t>7063055F-F00B-4788-BE25-0AF9148C3A78</t>
+  </si>
+  <si>
+    <t>3B6FC0DA-115F-46DA-8613-255B19BC0A3E</t>
+  </si>
+  <si>
+    <t>A4A7D7FA-23F9-4ADA-B643-10307BD31C8B</t>
+  </si>
+  <si>
+    <t>FLFLIIN2O</t>
+  </si>
+  <si>
+    <t>FLFLIICH4</t>
+  </si>
+  <si>
+    <t>CLFLIIN2O</t>
+  </si>
+  <si>
+    <t>CLFLIICH4</t>
+  </si>
+  <si>
+    <t>GLFLIIN2O</t>
+  </si>
+  <si>
+    <t>GLFLIICH4</t>
+  </si>
+  <si>
+    <t>WLOFLIIN2O</t>
+  </si>
+  <si>
+    <t>WLOFLIICH4</t>
+  </si>
+  <si>
+    <t>SEFLIIN2O</t>
+  </si>
+  <si>
+    <t>SEFLIICH4</t>
+  </si>
+  <si>
+    <t>FLCLIVN2O</t>
+  </si>
+  <si>
+    <t>GLCLIVN2O</t>
+  </si>
+  <si>
+    <t>WLCLIVN2O</t>
+  </si>
+  <si>
+    <t>SECLIVN2O</t>
+  </si>
+  <si>
+    <t>FLGLIVN2O</t>
+  </si>
+  <si>
+    <t>CLGLIVN2O</t>
+  </si>
+  <si>
+    <t>WLGLIVN2O</t>
+  </si>
+  <si>
+    <t>SEGLIVN2O</t>
+  </si>
+  <si>
+    <t>A60D8558-4AB5-444E-84C3-F697036626EB</t>
+  </si>
+  <si>
+    <t>C67D494D-213C-4FE2-B4F8-0AE6D51387D7</t>
+  </si>
+  <si>
+    <t>BD322158-494A-4BC0-AA2B-9821F925CB7E</t>
+  </si>
+  <si>
+    <t>WLPWLPIIN2O</t>
+  </si>
+  <si>
+    <t>WLOWLPIIN2O</t>
+  </si>
+  <si>
+    <t>FLWLPIIN2O</t>
+  </si>
+  <si>
+    <t>CLWLPIIN2O</t>
+  </si>
+  <si>
+    <t>GLWLPIIN2O</t>
+  </si>
+  <si>
+    <t>WLOWLOIIN2O</t>
+  </si>
+  <si>
+    <t>WLPWLOIIN2O</t>
+  </si>
+  <si>
+    <t>FLWLOIIN2O</t>
+  </si>
+  <si>
+    <t>CLWLOIIN2O</t>
+  </si>
+  <si>
+    <t>WLPWLPIICH4</t>
+  </si>
+  <si>
+    <t>WLOWLPIICH4</t>
+  </si>
+  <si>
+    <t>FLWLPIICH4</t>
+  </si>
+  <si>
+    <t>CLWLPIICH4</t>
+  </si>
+  <si>
+    <t>GLWLPIICH4</t>
+  </si>
+  <si>
+    <t>FLWLFIICH4</t>
+  </si>
+  <si>
+    <t>CLWLFIICH4</t>
+  </si>
+  <si>
+    <t>GLWLFIICH4</t>
+  </si>
+  <si>
+    <t>SEWLFIICH4</t>
+  </si>
+  <si>
+    <t>WLOWLOIICH4</t>
+  </si>
+  <si>
+    <t>WLPWLOIICH4</t>
+  </si>
+  <si>
+    <t>FLWLOIICH4</t>
+  </si>
+  <si>
+    <t>CLWLOIICH4</t>
+  </si>
+  <si>
+    <t>WLFWLFIICH4</t>
+  </si>
+  <si>
+    <t>OLWLFIICH4</t>
+  </si>
+  <si>
+    <t>GLWLOIIN2O</t>
+  </si>
+  <si>
+    <t>GLWLOIICH4</t>
+  </si>
+  <si>
+    <t>CLWLOLOSS</t>
   </si>
 </sst>
 </file>
@@ -770,7 +932,7 @@
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -789,6 +951,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -877,7 +1046,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -929,9 +1098,14 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -947,7 +1121,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1248,56 +1422,56 @@
   </sheetPr>
   <dimension ref="A3:AP130"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
-    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.6640625" customWidth="1"/>
-    <col min="5" max="5" width="6.5" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="6.5" customWidth="1"/>
-    <col min="9" max="9" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="10.85546875" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" customWidth="1"/>
+    <col min="9" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="6" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="22" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="28" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.1640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="5.5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:42" s="33" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="5" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:42" s="33" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:42" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1422,17 +1596,17 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
         <v>1</v>
       </c>
@@ -1485,7 +1659,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
         <v>2</v>
       </c>
@@ -1498,6 +1672,9 @@
       <c r="D10" s="4" t="s">
         <v>125</v>
       </c>
+      <c r="E10" s="41" t="s">
+        <v>241</v>
+      </c>
       <c r="F10" s="4" t="s">
         <v>126</v>
       </c>
@@ -1516,6 +1693,9 @@
       <c r="K10" s="4" t="s">
         <v>131</v>
       </c>
+      <c r="M10" s="41" t="s">
+        <v>237</v>
+      </c>
       <c r="O10" s="26" t="s">
         <v>132</v>
       </c>
@@ -1525,6 +1705,12 @@
       <c r="Q10" s="4" t="s">
         <v>134</v>
       </c>
+      <c r="S10" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="V10" s="41" t="s">
+        <v>239</v>
+      </c>
       <c r="W10" s="4" t="s">
         <v>135</v>
       </c>
@@ -1534,6 +1720,9 @@
       <c r="Y10" s="4" t="s">
         <v>137</v>
       </c>
+      <c r="Z10" s="41" t="s">
+        <v>246</v>
+      </c>
       <c r="AA10" s="4" t="s">
         <v>138</v>
       </c>
@@ -1546,6 +1735,9 @@
       <c r="AH10" s="4" t="s">
         <v>141</v>
       </c>
+      <c r="AI10" s="41" t="s">
+        <v>294</v>
+      </c>
       <c r="AJ10" s="4" t="s">
         <v>142</v>
       </c>
@@ -1558,14 +1750,17 @@
       <c r="AN10" s="4" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="11" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AP10" s="41" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
         <v>3</v>
       </c>
@@ -1585,7 +1780,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26">
         <v>4</v>
       </c>
@@ -1593,7 +1788,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
         <v>5</v>
       </c>
@@ -1649,7 +1844,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="15" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26">
         <v>6</v>
       </c>
@@ -1750,25 +1945,28 @@
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:42" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:36" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:36" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
         <v>7</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="20" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="43" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="20" spans="1:36" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <v>8</v>
       </c>
@@ -1776,52 +1974,158 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:32" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:36" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
       <c r="B21" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28">
         <v>9</v>
       </c>
       <c r="B24" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="U24" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="AF24" s="9" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="25" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C24" s="42" t="s">
+        <v>247</v>
+      </c>
+      <c r="D24" s="42" t="s">
+        <v>249</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>251</v>
+      </c>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42" t="s">
+        <v>253</v>
+      </c>
+      <c r="H24" s="42" t="s">
+        <v>255</v>
+      </c>
+      <c r="I24" s="42"/>
+      <c r="U24" s="42" t="s">
+        <v>268</v>
+      </c>
+      <c r="V24" s="42" t="s">
+        <v>269</v>
+      </c>
+      <c r="W24" s="42" t="s">
+        <v>270</v>
+      </c>
+      <c r="X24" s="42" t="s">
+        <v>271</v>
+      </c>
+      <c r="Y24" s="42" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z24" s="42"/>
+      <c r="AA24" s="42"/>
+      <c r="AB24" s="42"/>
+      <c r="AC24" s="42"/>
+      <c r="AD24" s="42"/>
+      <c r="AE24" s="42"/>
+      <c r="AF24" s="42" t="s">
+        <v>273</v>
+      </c>
+      <c r="AG24" s="42" t="s">
+        <v>274</v>
+      </c>
+      <c r="AH24" s="42" t="s">
+        <v>275</v>
+      </c>
+      <c r="AI24" s="42" t="s">
+        <v>276</v>
+      </c>
+      <c r="AJ24" s="42" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="25" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28">
         <v>10</v>
       </c>
       <c r="B25" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="U25" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="AF25" s="9" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="26" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C25" s="42" t="s">
+        <v>248</v>
+      </c>
+      <c r="D25" s="42" t="s">
+        <v>250</v>
+      </c>
+      <c r="E25" s="42" t="s">
+        <v>252</v>
+      </c>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42" t="s">
+        <v>254</v>
+      </c>
+      <c r="H25" s="42" t="s">
+        <v>256</v>
+      </c>
+      <c r="I25" s="42"/>
+      <c r="U25" s="42" t="s">
+        <v>277</v>
+      </c>
+      <c r="V25" s="42" t="s">
+        <v>278</v>
+      </c>
+      <c r="W25" s="42" t="s">
+        <v>279</v>
+      </c>
+      <c r="X25" s="42" t="s">
+        <v>280</v>
+      </c>
+      <c r="Y25" s="42" t="s">
+        <v>281</v>
+      </c>
+      <c r="Z25" s="42" t="s">
+        <v>290</v>
+      </c>
+      <c r="AA25" s="42" t="s">
+        <v>282</v>
+      </c>
+      <c r="AB25" s="42" t="s">
+        <v>283</v>
+      </c>
+      <c r="AC25" s="42" t="s">
+        <v>284</v>
+      </c>
+      <c r="AD25" s="42" t="s">
+        <v>285</v>
+      </c>
+      <c r="AE25" s="42" t="s">
+        <v>291</v>
+      </c>
+      <c r="AF25" s="42" t="s">
+        <v>286</v>
+      </c>
+      <c r="AG25" s="42" t="s">
+        <v>287</v>
+      </c>
+      <c r="AH25" s="42" t="s">
+        <v>288</v>
+      </c>
+      <c r="AI25" s="42" t="s">
+        <v>289</v>
+      </c>
+      <c r="AJ25" s="42" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="26" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="28"/>
       <c r="B26" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28">
         <v>11</v>
       </c>
@@ -1829,7 +2133,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="28">
         <v>12</v>
       </c>
@@ -1837,13 +2141,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
       <c r="B29" s="9" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28">
         <v>13</v>
       </c>
@@ -1851,7 +2155,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28">
         <v>14</v>
       </c>
@@ -1859,13 +2163,13 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:32" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="28"/>
       <c r="B32" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28">
         <v>15</v>
       </c>
@@ -1873,7 +2177,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="28">
         <v>16</v>
       </c>
@@ -1881,18 +2185,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="28"/>
       <c r="B35" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:38" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29">
         <v>17</v>
       </c>
@@ -1900,48 +2204,48 @@
         <v>32</v>
       </c>
       <c r="D38" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="J38" s="11" t="s">
         <v>201</v>
       </c>
-      <c r="E38" s="11" t="s">
+      <c r="K38" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="F38" s="11" t="s">
+      <c r="N38" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="H38" s="11" t="s">
+      <c r="P38" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="J38" s="11" t="s">
+      <c r="Q38" s="11" t="s">
         <v>205</v>
       </c>
-      <c r="K38" s="11" t="s">
+      <c r="R38" s="11" t="s">
         <v>206</v>
       </c>
-      <c r="N38" s="11" t="s">
+      <c r="T38" s="11" t="s">
         <v>207</v>
       </c>
-      <c r="P38" s="11" t="s">
+      <c r="AL38" s="11" t="s">
         <v>208</v>
       </c>
-      <c r="Q38" s="11" t="s">
-        <v>209</v>
-      </c>
-      <c r="R38" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="T38" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="AL38" s="11" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="40" spans="1:38" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:38" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:38" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:38" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>18</v>
       </c>
@@ -1949,15 +2253,42 @@
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="1:38" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>19</v>
       </c>
       <c r="B42" s="12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="43" spans="1:38" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="J42" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="K42" s="45" t="s">
+        <v>258</v>
+      </c>
+      <c r="L42" s="45" t="s">
+        <v>259</v>
+      </c>
+      <c r="M42" s="45"/>
+      <c r="N42" s="45" t="s">
+        <v>260</v>
+      </c>
+      <c r="O42" s="45"/>
+      <c r="P42" s="45" t="s">
+        <v>261</v>
+      </c>
+      <c r="Q42" s="45" t="s">
+        <v>262</v>
+      </c>
+      <c r="R42" s="45" t="s">
+        <v>263</v>
+      </c>
+      <c r="S42" s="45"/>
+      <c r="T42" s="45" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="43" spans="1:38" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>20</v>
       </c>
@@ -1965,12 +2296,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:38" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:38" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:38" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:38" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="31">
         <v>21</v>
       </c>
@@ -1978,89 +2309,113 @@
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:38" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:38" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31">
         <v>22</v>
       </c>
       <c r="B47" s="13" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="48" spans="1:38" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="44" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="48" spans="1:38" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="31">
         <v>23</v>
       </c>
       <c r="B48" s="13" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="44" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
       <c r="B49" s="13" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C49" s="44"/>
+    </row>
+    <row r="50" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
-    </row>
-    <row r="51" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C50" s="44"/>
+    </row>
+    <row r="51" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="31">
         <v>24</v>
       </c>
       <c r="B51" s="13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C51" s="44"/>
+      <c r="N51" s="44" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="31">
         <v>25</v>
       </c>
       <c r="B52" s="13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C52" s="44" t="s">
+        <v>245</v>
+      </c>
+      <c r="N52" s="44" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="31">
         <v>26</v>
       </c>
       <c r="B53" s="13" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C53" s="44" t="s">
+        <v>244</v>
+      </c>
+      <c r="N53" s="44" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="13" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="13" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="13" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="13" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="32" t="s">
         <v>51</v>
       </c>
       <c r="B61" s="32"/>
       <c r="C61" s="32"/>
     </row>
-    <row r="62" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="32">
         <v>27</v>
       </c>
@@ -2068,10 +2423,10 @@
         <v>59</v>
       </c>
       <c r="C62" s="32" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="32">
         <v>28</v>
       </c>
@@ -2079,17 +2434,17 @@
         <v>60</v>
       </c>
       <c r="C63" s="32" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="32"/>
       <c r="B64" s="32" t="s">
         <v>61</v>
       </c>
       <c r="C64" s="32"/>
     </row>
-    <row r="65" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="32">
         <v>29</v>
       </c>
@@ -2097,10 +2452,10 @@
         <v>62</v>
       </c>
       <c r="C65" s="32" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="32">
         <v>30</v>
       </c>
@@ -2108,17 +2463,17 @@
         <v>63</v>
       </c>
       <c r="C66" s="32" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="32"/>
       <c r="B67" s="32" t="s">
         <v>64</v>
       </c>
       <c r="C67" s="32"/>
     </row>
-    <row r="68" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="32">
         <v>31</v>
       </c>
@@ -2126,10 +2481,10 @@
         <v>65</v>
       </c>
       <c r="C68" s="32" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="32">
         <v>32</v>
       </c>
@@ -2137,265 +2492,265 @@
         <v>66</v>
       </c>
       <c r="C69" s="32" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="32"/>
       <c r="B70" s="32" t="s">
         <v>67</v>
       </c>
       <c r="C70" s="32"/>
     </row>
-    <row r="71" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="32"/>
       <c r="B71" s="32" t="s">
         <v>55</v>
       </c>
       <c r="C71" s="32"/>
     </row>
-    <row r="73" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B76" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="78" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="79" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="80" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="81" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="82" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="83" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="16" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="86" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B87" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="88" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="18" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="91" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="92" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B92" s="9" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="94" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="19" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="9" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="97" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="19" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="98" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B98" s="9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="99" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="101" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="102" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B102" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="103" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="105" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A105" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="106" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:2" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B106" s="20" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="109" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B109" s="12" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="110" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B110" s="12" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="111" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:2" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B111" s="21" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="113" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="114" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B114" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="115" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B115" s="13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="116" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B116" s="13" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="117" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B117" s="22" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="118" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="119" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B119" s="13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="120" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="13" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="121" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="122" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B122" s="22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="124" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A124" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="125" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B125" s="14" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="126" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B126" s="14" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="127" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:2" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B127" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="128" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:2" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B128" s="23" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="130" spans="1:1" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:1" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A130" s="24" t="s">
         <v>58</v>
       </c>
@@ -2417,15 +2772,15 @@
       <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" style="25" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="25" customWidth="1"/>
     <col min="2" max="2" width="30" style="25" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" style="25" customWidth="1"/>
-    <col min="4" max="16384" width="8.83203125" style="25"/>
+    <col min="3" max="3" width="11.28515625" style="25" customWidth="1"/>
+    <col min="4" max="16384" width="8.85546875" style="25"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:64" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:64" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D3" s="1">
         <v>1990</v>
       </c>
@@ -2670,22 +3025,22 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="5" spans="1:64" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:64" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
         <v>1</v>
       </c>
@@ -2696,7 +3051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="26">
         <v>2</v>
       </c>
@@ -2707,7 +3062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="5" t="s">
         <v>6</v>
@@ -2716,7 +3071,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26">
         <v>3</v>
       </c>
@@ -2727,7 +3082,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26">
         <v>4</v>
       </c>
@@ -2738,7 +3093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26">
         <v>5</v>
       </c>
@@ -2749,7 +3104,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26">
         <v>6</v>
       </c>
@@ -2760,7 +3115,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:64" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>11</v>
       </c>
@@ -2768,12 +3123,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="27">
         <v>7</v>
       </c>
@@ -2784,7 +3139,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="27">
         <v>8</v>
       </c>
@@ -2795,7 +3150,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="27"/>
       <c r="B21" s="8" t="s">
         <v>11</v>
@@ -2804,12 +3159,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28">
         <v>9</v>
       </c>
@@ -2820,7 +3175,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28">
         <v>10</v>
       </c>
@@ -2831,7 +3186,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="28"/>
       <c r="B26" s="9" t="s">
         <v>20</v>
@@ -2840,7 +3195,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28">
         <v>11</v>
       </c>
@@ -2851,7 +3206,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="28">
         <v>12</v>
       </c>
@@ -2862,7 +3217,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28"/>
       <c r="B29" s="9" t="s">
         <v>24</v>
@@ -2871,7 +3226,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28">
         <v>13</v>
       </c>
@@ -2882,7 +3237,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28">
         <v>14</v>
       </c>
@@ -2893,13 +3248,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="28"/>
       <c r="B32" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28">
         <v>15</v>
       </c>
@@ -2910,7 +3265,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="28">
         <v>16</v>
       </c>
@@ -2921,7 +3276,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="28"/>
       <c r="B35" s="9" t="s">
         <v>30</v>
@@ -2930,12 +3285,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="29">
         <v>17</v>
       </c>
@@ -2946,12 +3301,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="30">
         <v>18</v>
       </c>
@@ -2962,7 +3317,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="30">
         <v>19</v>
       </c>
@@ -2973,7 +3328,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <v>20</v>
       </c>
@@ -2984,12 +3339,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="31">
         <v>21</v>
       </c>
@@ -3000,7 +3355,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="31">
         <v>22</v>
       </c>
@@ -3011,7 +3366,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="31">
         <v>23</v>
       </c>
@@ -3022,7 +3377,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="31"/>
       <c r="B49" s="13" t="s">
         <v>42</v>
@@ -3031,10 +3386,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="50" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="31"/>
     </row>
-    <row r="51" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="31">
         <v>24</v>
       </c>
@@ -3045,7 +3400,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="52" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="31">
         <v>25</v>
       </c>
@@ -3056,7 +3411,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="53" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="31">
         <v>26</v>
       </c>
@@ -3067,7 +3422,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="13" t="s">
         <v>46</v>
       </c>
@@ -3075,8 +3430,8 @@
         <v>21</v>
       </c>
     </row>
-    <row r="55" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="13" t="s">
         <v>47</v>
       </c>
@@ -3084,7 +3439,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="57" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B57" s="13" t="s">
         <v>48</v>
       </c>
@@ -3092,7 +3447,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B58" s="13" t="s">
         <v>49</v>
       </c>
@@ -3100,7 +3455,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B59" s="13" t="s">
         <v>50</v>
       </c>
@@ -3108,14 +3463,14 @@
         <v>21</v>
       </c>
     </row>
-    <row r="61" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="32" t="s">
         <v>51</v>
       </c>
       <c r="B61" s="32"/>
       <c r="C61" s="32"/>
     </row>
-    <row r="62" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="32">
         <v>27</v>
       </c>
@@ -3126,7 +3481,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="63" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="32">
         <v>28</v>
       </c>
@@ -3137,7 +3492,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="64" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="32"/>
       <c r="B64" s="32" t="s">
         <v>61</v>
@@ -3146,7 +3501,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="65" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="32">
         <v>29</v>
       </c>
@@ -3157,7 +3512,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="66" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="32">
         <v>30</v>
       </c>
@@ -3168,7 +3523,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="67" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="32"/>
       <c r="B67" s="32" t="s">
         <v>64</v>
@@ -3177,7 +3532,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="68" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="32">
         <v>31</v>
       </c>
@@ -3188,7 +3543,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="69" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="32">
         <v>32</v>
       </c>
@@ -3199,7 +3554,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="70" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="32"/>
       <c r="B70" s="32" t="s">
         <v>67</v>
@@ -3208,7 +3563,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="71" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="32"/>
       <c r="B71" s="32" t="s">
         <v>55</v>
@@ -3217,22 +3572,22 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B77" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B78" s="5" t="s">
         <v>3</v>
       </c>
@@ -3240,7 +3595,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="79" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
         <v>5</v>
       </c>
@@ -3248,7 +3603,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B80" s="5" t="s">
         <v>6</v>
       </c>
@@ -3256,7 +3611,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="81" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B81" s="6" t="s">
         <v>7</v>
       </c>
@@ -3264,7 +3619,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="82" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B82" s="6" t="s">
         <v>8</v>
       </c>
@@ -3272,7 +3627,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="83" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B83" s="4" t="s">
         <v>9</v>
       </c>
@@ -3280,7 +3635,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="84" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B84" s="4" t="s">
         <v>10</v>
       </c>
@@ -3288,7 +3643,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="85" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B85" s="16" t="s">
         <v>11</v>
       </c>
@@ -3296,12 +3651,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="87" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B88" s="8" t="s">
         <v>13</v>
       </c>
@@ -3309,7 +3664,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="89" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B89" s="8" t="s">
         <v>15</v>
       </c>
@@ -3317,7 +3672,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="90" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:3" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B90" s="18" t="s">
         <v>11</v>
       </c>
@@ -3325,12 +3680,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="92" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="93" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B93" s="9" t="s">
         <v>17</v>
       </c>
@@ -3338,7 +3693,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="94" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B94" s="9" t="s">
         <v>18</v>
       </c>
@@ -3346,7 +3701,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="95" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B95" s="19" t="s">
         <v>20</v>
       </c>
@@ -3354,7 +3709,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="96" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B96" s="9" t="s">
         <v>22</v>
       </c>
@@ -3362,7 +3717,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B97" s="9" t="s">
         <v>23</v>
       </c>
@@ -3370,7 +3725,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="98" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B98" s="19" t="s">
         <v>24</v>
       </c>
@@ -3378,7 +3733,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B99" s="9" t="s">
         <v>25</v>
       </c>
@@ -3386,7 +3741,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B100" s="9" t="s">
         <v>26</v>
       </c>
@@ -3394,7 +3749,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="101" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B101" s="19" t="s">
         <v>27</v>
       </c>
@@ -3402,7 +3757,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B102" s="9" t="s">
         <v>28</v>
       </c>
@@ -3410,7 +3765,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:3" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B103" s="9" t="s">
         <v>29</v>
       </c>
@@ -3418,7 +3773,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="104" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B104" s="19" t="s">
         <v>30</v>
       </c>
@@ -3426,12 +3781,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="106" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="107" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B107" s="20" t="s">
         <v>32</v>
       </c>
@@ -3439,12 +3794,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="109" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A109" s="12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="110" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B110" s="12" t="s">
         <v>34</v>
       </c>
@@ -3452,7 +3807,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="111" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B111" s="12" t="s">
         <v>35</v>
       </c>
@@ -3460,7 +3815,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="112" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B112" s="21" t="s">
         <v>36</v>
       </c>
@@ -3468,12 +3823,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="114" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="115" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B115" s="13" t="s">
         <v>38</v>
       </c>
@@ -3481,7 +3836,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="116" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B116" s="13" t="s">
         <v>40</v>
       </c>
@@ -3489,7 +3844,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="117" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B117" s="13" t="s">
         <v>41</v>
       </c>
@@ -3497,7 +3852,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="118" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B118" s="22" t="s">
         <v>42</v>
       </c>
@@ -3505,8 +3860,8 @@
         <v>56</v>
       </c>
     </row>
-    <row r="119" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="120" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B120" s="13" t="s">
         <v>43</v>
       </c>
@@ -3514,7 +3869,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="121" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B121" s="13" t="s">
         <v>44</v>
       </c>
@@ -3522,7 +3877,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="122" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:3" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B122" s="13" t="s">
         <v>45</v>
       </c>
@@ -3530,7 +3885,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="123" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B123" s="22" t="s">
         <v>46</v>
       </c>
@@ -3538,12 +3893,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="125" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A125" s="14" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="126" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B126" s="14" t="s">
         <v>52</v>
       </c>
@@ -3551,7 +3906,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="127" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B127" s="14" t="s">
         <v>53</v>
       </c>
@@ -3559,7 +3914,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="128" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:3" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B128" s="14" t="s">
         <v>54</v>
       </c>
@@ -3567,7 +3922,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="129" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:3" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B129" s="23" t="s">
         <v>55</v>
       </c>
@@ -3575,7 +3930,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="131" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="24" t="s">
         <v>58</v>
       </c>
@@ -3589,30 +3944,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C0CE37D-972E-8C46-9914-72567F0F6FE5}">
   <dimension ref="A1:BM34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="4" max="64" width="10.1640625" customWidth="1"/>
-    <col min="65" max="65" width="8.83203125" style="34"/>
+    <col min="4" max="64" width="10.140625" customWidth="1"/>
+    <col min="65" max="65" width="8.85546875" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:65" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="33" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D1" s="33">
         <v>1990</v>
@@ -3859,12 +4214,12 @@
       </c>
       <c r="BM1" s="37"/>
     </row>
-    <row r="2" spans="1:65" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:65" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="33" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" t="s">
         <v>234</v>
-      </c>
-      <c r="C2" t="s">
-        <v>238</v>
       </c>
       <c r="D2" s="40"/>
       <c r="E2" s="40"/>
@@ -3929,12 +4284,12 @@
       <c r="BL2" s="40"/>
       <c r="BM2" s="37"/>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D3" s="39"/>
       <c r="E3" s="39"/>
@@ -3998,12 +4353,12 @@
       <c r="BK3" s="36"/>
       <c r="BL3" s="36"/>
     </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D4" s="39"/>
       <c r="E4" s="39"/>
@@ -4067,12 +4422,12 @@
       <c r="BK4" s="39"/>
       <c r="BL4" s="39"/>
     </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D5" s="39"/>
       <c r="E5" s="39"/>
@@ -4136,12 +4491,12 @@
       <c r="BK5" s="39"/>
       <c r="BL5" s="39"/>
     </row>
-    <row r="6" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C6" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D6" s="39"/>
       <c r="E6" s="35"/>
@@ -4195,12 +4550,12 @@
       <c r="BK6" s="35"/>
       <c r="BL6" s="35"/>
     </row>
-    <row r="7" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D7" s="39"/>
       <c r="E7" s="39"/>
@@ -4264,12 +4619,12 @@
       <c r="BK7" s="39"/>
       <c r="BL7" s="39"/>
     </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C8" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D8" s="39"/>
       <c r="E8" s="39"/>
@@ -4333,12 +4688,12 @@
       <c r="BK8" s="39"/>
       <c r="BL8" s="39"/>
     </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C9" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D9" s="39"/>
       <c r="E9" s="35"/>
@@ -4392,12 +4747,12 @@
       <c r="BK9" s="35"/>
       <c r="BL9" s="35"/>
     </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>81</v>
       </c>
       <c r="C10" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D10" s="39"/>
       <c r="E10" s="39"/>
@@ -4461,12 +4816,12 @@
       <c r="BK10" s="39"/>
       <c r="BL10" s="39"/>
     </row>
-    <row r="11" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C11" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D11" s="39"/>
       <c r="E11" s="39"/>
@@ -4530,12 +4885,12 @@
       <c r="BK11" s="39"/>
       <c r="BL11" s="39"/>
     </row>
-    <row r="12" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C12" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D12" s="39"/>
       <c r="E12" s="35"/>
@@ -4589,12 +4944,12 @@
       <c r="BK12" s="35"/>
       <c r="BL12" s="35"/>
     </row>
-    <row r="13" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C13" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D13" s="39"/>
       <c r="E13" s="39"/>
@@ -4658,12 +5013,12 @@
       <c r="BK13" s="39"/>
       <c r="BL13" s="39"/>
     </row>
-    <row r="14" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C14" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D14" s="39"/>
       <c r="E14" s="39"/>
@@ -4727,12 +5082,12 @@
       <c r="BK14" s="39"/>
       <c r="BL14" s="39"/>
     </row>
-    <row r="15" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C15" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D15" s="39"/>
       <c r="E15" s="35"/>
@@ -4786,12 +5141,12 @@
       <c r="BK15" s="35"/>
       <c r="BL15" s="35"/>
     </row>
-    <row r="16" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>103</v>
       </c>
       <c r="C16" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D16" s="39"/>
       <c r="E16" s="39"/>
@@ -4855,12 +5210,12 @@
       <c r="BK16" s="39"/>
       <c r="BL16" s="39"/>
     </row>
-    <row r="17" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C17" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D17" s="39"/>
       <c r="E17" s="39"/>
@@ -4924,12 +5279,12 @@
       <c r="BK17" s="39"/>
       <c r="BL17" s="39"/>
     </row>
-    <row r="18" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:65" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C18" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D18" s="35"/>
       <c r="E18" s="35"/>
@@ -4993,15 +5348,15 @@
       <c r="BK18" s="35"/>
       <c r="BL18" s="35"/>
     </row>
-    <row r="19" spans="1:65" s="33" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:65" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="33" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B19" s="33" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C19" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D19"/>
       <c r="E19"/>
@@ -5066,71 +5421,71 @@
       <c r="BL19"/>
       <c r="BM19" s="37"/>
     </row>
-    <row r="20" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>76</v>
       </c>
       <c r="C20" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="21" spans="1:65" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="21" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>82</v>
       </c>
       <c r="C21" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="22" spans="1:65" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="22" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>89</v>
       </c>
       <c r="C22" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="23" spans="1:65" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>93</v>
       </c>
       <c r="C23" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="24" spans="1:65" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="24" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>100</v>
       </c>
       <c r="C24" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="25" spans="1:65" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="25" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>104</v>
       </c>
       <c r="C25" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="26" spans="1:65" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="26" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C26" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="27" spans="1:65" s="33" customFormat="1" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="27" spans="1:65" s="33" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="33" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C27" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D27"/>
       <c r="E27"/>
@@ -5195,60 +5550,60 @@
       <c r="BL27"/>
       <c r="BM27" s="37"/>
     </row>
-    <row r="28" spans="1:65" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="29" spans="1:65" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="29" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>71</v>
       </c>
       <c r="C29" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="30" spans="1:65" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="30" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>72</v>
       </c>
       <c r="C30" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="31" spans="1:65" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C31" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="32" spans="1:65" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="32" spans="1:65" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>73</v>
       </c>
       <c r="C32" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>74</v>
       </c>
       <c r="C33" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.2">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C34" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>